<commit_message>
More changes to Class 3
</commit_message>
<xml_diff>
--- a/Class3/t-tests and ANOVA with Excel.xlsx
+++ b/Class3/t-tests and ANOVA with Excel.xlsx
@@ -708,7 +708,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -733,15 +733,15 @@
       </c>
       <c r="B2">
         <f ca="1">_xlfn.NORM.INV(RAND(), 100, 15)</f>
-        <v>96.004581007824257</v>
+        <v>79.271370843304652</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:D2" ca="1" si="0">_xlfn.NORM.INV(RAND(), 100, 15)</f>
-        <v>114.11857721887384</v>
+        <v>91.176368839596549</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>120.16089792883484</v>
+        <v>81.052727820605071</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16.8" x14ac:dyDescent="0.55000000000000004">
@@ -750,15 +750,15 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:D11" ca="1" si="1">_xlfn.NORM.INV(RAND(), 100, 15)</f>
-        <v>111.70291090087586</v>
+        <v>94.651563286116186</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="1"/>
-        <v>92.64112136874553</v>
+        <v>93.926206011153951</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>121.60057365670963</v>
+        <v>96.590475715224301</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -768,15 +768,15 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>84.597747890186213</v>
+        <v>95.88641161140923</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="1"/>
-        <v>117.6081613465924</v>
+        <v>98.946874128483373</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
-        <v>99.306359409389017</v>
+        <v>106.26344722438049</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -786,15 +786,15 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>94.03789939249485</v>
+        <v>83.97959623422706</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="1"/>
-        <v>73.950869673986233</v>
+        <v>103.75774051460778</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
-        <v>95.23925535180382</v>
+        <v>88.614740700205175</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -803,15 +803,15 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>96.433491903239968</v>
+        <v>121.70101328088261</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>104.12447787618767</v>
+        <v>94.968804780872986</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
-        <v>109.05634028510129</v>
+        <v>116.30028569148031</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -820,15 +820,15 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>71.466729465110646</v>
+        <v>120.5833163372272</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>112.03679495334528</v>
+        <v>110.12163733145218</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
-        <v>62.871762224249949</v>
+        <v>121.19637538088102</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -837,15 +837,15 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>115.64400230241235</v>
+        <v>110.63264134095721</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>105.14875610655271</v>
+        <v>108.39706277572779</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>72.204490145416116</v>
+        <v>95.200308002587562</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -854,15 +854,15 @@
       </c>
       <c r="B9">
         <f ca="1">_xlfn.NORM.INV(RAND(), 100, 15)</f>
-        <v>122.04223758910651</v>
+        <v>96.572284875389656</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>89.417129550289658</v>
+        <v>96.286173924489603</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
-        <v>75.979506434253111</v>
+        <v>112.57305353087372</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -871,15 +871,15 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>84.543412574019953</v>
+        <v>91.537873302367771</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>85.587125892012338</v>
+        <v>93.008256907345967</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>111.638738862723</v>
+        <v>93.93710552390624</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -888,15 +888,15 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>79.050139692670626</v>
+        <v>102.20893393214814</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>118.40907772748012</v>
+        <v>104.21642293762564</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
-        <v>107.94538334375372</v>
+        <v>94.732406469439596</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -905,15 +905,15 @@
       </c>
       <c r="B12">
         <f ca="1">AVERAGE(B2:B11)</f>
-        <v>95.552315271794129</v>
+        <v>99.702500504402977</v>
       </c>
       <c r="C12">
         <f t="shared" ref="C12:D12" ca="1" si="2">AVERAGE(C2:C11)</f>
-        <v>101.30420917140658</v>
+        <v>99.480554815135591</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="2"/>
-        <v>97.600330764223457</v>
+        <v>100.64609260595836</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -922,15 +922,15 @@
       </c>
       <c r="B13">
         <f ca="1">_xlfn.STDEV.S(B2:B11)</f>
-        <v>16.543356541448919</v>
+        <v>14.247291702980105</v>
       </c>
       <c r="C13">
         <f ca="1">_xlfn.STDEV.S(C2:C11)</f>
-        <v>15.173477987907285</v>
+        <v>6.7165237701346792</v>
       </c>
       <c r="D13">
         <f t="shared" ref="C13:D13" ca="1" si="3">_xlfn.STDEV.P(D2:D11)</f>
-        <v>19.614523873301572</v>
+        <v>12.230760872050199</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -950,45 +950,45 @@
       </c>
       <c r="B17">
         <f ca="1">(B12-C12)/SQRT(B13^2/(10)+C13^2/(10))</f>
-        <v>-0.81027292441143306</v>
+        <v>4.4559052462961435E-2</v>
       </c>
       <c r="C17">
         <f ca="1">2*(1-_xlfn.T.DIST(ABS(B17), 9, TRUE))</f>
-        <v>0.43868225815398865</v>
+        <v>0.96543177418536907</v>
       </c>
       <c r="D17">
         <f ca="1">2*(1-_xlfn.T.DIST(ABS(B17), 8, TRUE))</f>
-        <v>0.44121800178527537</v>
+        <v>0.96555094039576361</v>
       </c>
       <c r="F17" t="s">
         <v>16</v>
       </c>
       <c r="G17">
         <f ca="1">(B12-D12)/SQRT(B13^2/(10)+F13^2/(10))</f>
-        <v>-0.39148002542057203</v>
+        <v>-0.20943631149461014</v>
       </c>
       <c r="H17">
         <f ca="1">2*(1-_xlfn.T.DIST(ABS(G17), 9, TRUE))</f>
-        <v>0.7045497351073795</v>
+        <v>0.83877158159755782</v>
       </c>
       <c r="I17">
         <f ca="1">2*(1-_xlfn.T.DIST(ABS(G17), 8, TRUE))</f>
-        <v>0.70566331647785407</v>
+        <v>0.83934258820536201</v>
       </c>
       <c r="K17" t="s">
         <v>16</v>
       </c>
       <c r="L17">
         <f ca="1">(C12-D12)/SQRT(C13^2/(10)+D13^2/(10))</f>
-        <v>0.47231515543435421</v>
+        <v>-0.26414342898970383</v>
       </c>
       <c r="M17">
         <f ca="1">2*(1-_xlfn.T.DIST(ABS(L17), 9, TRUE))</f>
-        <v>0.6479444027157204</v>
+        <v>0.79761843026901147</v>
       </c>
       <c r="N17">
         <f ca="1">2*(1-_xlfn.T.DIST(ABS(L17), 8, TRUE))</f>
-        <v>0.64931770852167081</v>
+        <v>0.79834658015971693</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1040,19 +1040,19 @@
     <row r="21" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <f ca="1">_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
-        <v>0.42844413086089894</v>
+        <v>0.96514578412094165</v>
       </c>
       <c r="B21">
         <f ca="1">_xlfn.T.INV(1-A21, 8)</f>
-        <v>0.18624550998882056</v>
+        <v>-2.0928500771176535</v>
       </c>
       <c r="F21">
         <f ca="1">_xlfn.T.TEST(B2:B11,D2:D11,2,3)</f>
-        <v>0.80967834915328418</v>
+        <v>0.87833478054249503</v>
       </c>
       <c r="K21">
         <f ca="1">_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
-        <v>0.6538303243500414</v>
+        <v>0.80365512991253885</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1078,22 +1078,22 @@
       </c>
       <c r="B23">
         <f ca="1">DEVSQ(B2:B11)+DEVSQ(C2:C11)+DEVSQ(D2:D11)</f>
-        <v>8382.549186926266</v>
+        <v>3728.7882269140719</v>
       </c>
       <c r="C23">
         <v>27</v>
       </c>
       <c r="D23">
         <f ca="1">B23/C23</f>
-        <v>310.46478470097281</v>
+        <v>138.10326766348413</v>
       </c>
       <c r="E23">
         <f ca="1">D25/D23</f>
-        <v>0.27376892462455138</v>
+        <v>2.77341287648829E-2</v>
       </c>
       <c r="F23">
         <f ca="1">_xlfn.F.DIST.RT(E25, C25,C23)</f>
-        <v>0.76259362812268572</v>
+        <v>0.97267460274865147</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1102,14 +1102,14 @@
       </c>
       <c r="B24">
         <f ca="1">DEVSQ(B2:D11)</f>
-        <v>8552.540407409022</v>
+        <v>3736.4485745305328</v>
       </c>
       <c r="C24">
         <v>29</v>
       </c>
       <c r="D24">
         <f t="shared" ref="D24:D25" ca="1" si="4">B24/C24</f>
-        <v>294.91518646238006</v>
+        <v>128.8430542941563</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -1118,26 +1118,26 @@
       </c>
       <c r="B25">
         <f ca="1">10*((B12-AVERAGE(B2:D11))^2+(C12-AVERAGE(B2:D11))^2+(D12-AVERAGE(B2:D11))^2)</f>
-        <v>169.9912204827564</v>
+        <v>7.6603476164603155</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25">
         <f ca="1">B25/C25</f>
-        <v>84.995610241378202</v>
+        <v>3.8301738082301577</v>
       </c>
       <c r="E25">
         <f ca="1">D25/D23</f>
-        <v>0.27376892462455138</v>
+        <v>2.77341287648829E-2</v>
       </c>
       <c r="F25">
         <f ca="1">1-_xlfn.F.DIST(E25,C25,C23, TRUE)</f>
-        <v>0.76259362812268572</v>
+        <v>0.97267460274865147</v>
       </c>
       <c r="G25">
         <f ca="1">_xlfn.F.DIST.RT(E25,C25,C23)</f>
-        <v>0.76259362812268572</v>
+        <v>0.97267460274865147</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.55000000000000004">

</xml_diff>